<commit_message>
Update Converting program and data to get more variables 2
</commit_message>
<xml_diff>
--- a/Artifact Experiment/Daisuke 25-7-18/2018-07-25 16.28.00 PRESENTATION DAISUKE LEFT HAND NOT MOVING/EDASCLMEAN.xlsx
+++ b/Artifact Experiment/Daisuke 25-7-18/2018-07-25 16.28.00 PRESENTATION DAISUKE LEFT HAND NOT MOVING/EDASCLMEAN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\TPS 2A\Stage 2A\TNO\cleaning signal\stimuli\Daisuke 25-7-18\2018-07-25 16.28.00 PRESENTATION DAISUKE LEFT HAND NOT MOVING\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF93B0C-1479-48B3-BCBA-8F1045A92EC4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66E3493-4817-49AE-8BB4-E8A8CDE84475}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7848" xr2:uid="{DFCB8BB5-4D67-4BA6-B529-9DDEBB73C135}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7848" xr2:uid="{39D637FE-F363-480F-B4F6-3DD3B4572284}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -371,7 +371,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF1B7504-543D-49CE-ADBF-ADDFF0FBE965}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F243AC0-C477-4B05-82C6-F6ABB3AFBC29}">
   <dimension ref="A1:B44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">

</xml_diff>